<commit_message>
1 add testcase(face_detect) 2 enhance clus_face update db
</commit_message>
<xml_diff>
--- a/doc/testcase.xlsx
+++ b/doc/testcase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>No.</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -71,6 +71,82 @@
   </si>
   <si>
     <t>i7-7700HQ 2.8G 8core, 16G Mem</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3#</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>width</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>height</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>detect sec</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>file size</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>129 pics football</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>test machine</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.23.71</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intel(R) Xeon(R) CPU E5-2620 v2 @ 2.10GHz</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>24core</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mem</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>32GB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1MB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>16MB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>100k-300kB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>20k-90k</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>60k-300k</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -121,11 +197,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,16 +507,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H11"/>
+  <dimension ref="B2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="24.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.375" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
     <col min="6" max="6" width="12.875" style="1" customWidth="1"/>
@@ -557,6 +636,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1">
+        <v>23.71</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -566,12 +653,276 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.25" customWidth="1"/>
+    <col min="3" max="3" width="15.625" customWidth="1"/>
+    <col min="5" max="5" width="11.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>7952</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5304</v>
+      </c>
+      <c r="E3" s="2">
+        <v>37</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>8640</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5760</v>
+      </c>
+      <c r="E4" s="2">
+        <v>43</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1920</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1080</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1280</v>
+      </c>
+      <c r="D6" s="2">
+        <v>720</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>720</v>
+      </c>
+      <c r="D7" s="2">
+        <v>480</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>